<commit_message>
maintenance for the first deployment has been completed
</commit_message>
<xml_diff>
--- a/server/files/template-files/Disiplin_Kurulu_Kararlari_Aktarma_Dosyasi_v1.0.xlsx
+++ b/server/files/template-files/Disiplin_Kurulu_Kararlari_Aktarma_Dosyasi_v1.0.xlsx
@@ -1426,8 +1426,8 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="5"/>

</xml_diff>